<commit_message>
Sprint and Product Backlog 1
</commit_message>
<xml_diff>
--- a/Documents/Product-Backlog .xlsx
+++ b/Documents/Product-Backlog .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayadharshini.n\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4489046-4F00-4018-ABBD-81E8AB677609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CDE0BF-21E3-4DDA-9C98-16F07194568F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -579,18 +579,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -614,6 +602,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1489,12 +1492,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="9"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1530,10 +1533,10 @@
       <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1593,12 +1596,12 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="8"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -2207,7 +2210,7 @@
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="18"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2994,7 +2997,7 @@
   <dimension ref="A3:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3004,214 +3007,274 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="22" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="23">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="19">
         <v>45008</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="19">
         <v>45009</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="19">
         <v>45012</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="19">
+        <v>45013</v>
+      </c>
+      <c r="G4" s="19">
         <v>45014</v>
       </c>
-      <c r="G4" s="23">
-        <v>45014</v>
-      </c>
-      <c r="H4" s="23">
+      <c r="H4" s="19">
         <v>45015</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="20">
         <v>1</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <v>2</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="20">
         <v>3</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="20">
         <v>4</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="20">
         <v>5</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="15">
         <v>1</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="D6" s="26">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26">
+        <v>5</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="15">
         <v>2</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="26">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26">
+        <v>6</v>
+      </c>
+      <c r="E7" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="15">
         <v>3</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="C8" s="26">
+        <v>6</v>
+      </c>
+      <c r="D8" s="26">
+        <v>6.5</v>
+      </c>
+      <c r="E8" s="26">
+        <v>5</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="15">
         <v>4</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="C9" s="26">
+        <v>5</v>
+      </c>
+      <c r="D9" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E9" s="26">
+        <v>6</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="15">
         <v>5</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="C10" s="26">
+        <v>5</v>
+      </c>
+      <c r="D10" s="26">
+        <v>6</v>
+      </c>
+      <c r="E10" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="15">
         <v>6</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="26">
+        <v>5</v>
+      </c>
+      <c r="D11" s="26">
+        <v>5</v>
+      </c>
+      <c r="E11" s="26">
+        <v>6</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="15">
         <v>7</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="C12" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="D12" s="26">
+        <v>6</v>
+      </c>
+      <c r="E12" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="15">
         <v>8</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="C13" s="26">
+        <v>6</v>
+      </c>
+      <c r="D13" s="26">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26">
+        <v>8</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="15">
         <v>9</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="D14" s="26">
+        <v>7</v>
+      </c>
+      <c r="E14" s="26">
+        <v>8</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="15">
         <v>10</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="26">
+        <v>5</v>
+      </c>
+      <c r="D15" s="26">
+        <v>5</v>
+      </c>
+      <c r="E15" s="26">
+        <v>6</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>